<commit_message>
Update Excel Sheet for OMOs
</commit_message>
<xml_diff>
--- a/data/FED_OpenMarket_Operations.xlsx
+++ b/data/FED_OpenMarket_Operations.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="1480">
   <si>
     <t>Date</t>
   </si>
@@ -4455,14 +4455,21 @@
   </si>
   <si>
     <t>Scheduled</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>20y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -4493,12 +4500,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -4779,21 +4787,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4813,371 +4822,385 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>1479</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>37236</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>37566</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>37797</v>
       </c>
-      <c r="B2" s="4">
-        <f>VLOOKUP(A2,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B4" s="4">
+        <f>VLOOKUP(A4,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
         <v>0.01</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D4" s="2">
         <v>0.01</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E4" s="2">
         <f>-25/10000</f>
         <v>-2.5000000000000001E-3</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F4" s="2">
         <f>-25/10000</f>
         <v>-2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>38168</v>
-      </c>
-      <c r="B3" s="4">
-        <f>VLOOKUP(A3,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <f>25/10000</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="F3" s="2">
-        <f>25/10000</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>38209</v>
-      </c>
-      <c r="B4" s="4">
-        <f>VLOOKUP(A4,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <f>25/10000</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="F4" s="2">
-        <f>25/10000</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>38251</v>
       </c>
       <c r="B5" s="4">
         <f>VLOOKUP(A5,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>1.7500000000000002E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>1.7500000000000002E-2</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E5" s="2">
-        <f>25/10000</f>
+        <f t="shared" ref="E5:F16" si="0">25/10000</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F5" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>38301</v>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>38209</v>
       </c>
       <c r="B6" s="4">
         <f>VLOOKUP(A6,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D6" s="2">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E6" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F6" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>38335</v>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>38251</v>
       </c>
       <c r="B7" s="4">
         <f>VLOOKUP(A7,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>2.2499999999999999E-2</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>2.2499999999999999E-2</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="E7" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F7" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>38385</v>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>38301</v>
       </c>
       <c r="B8" s="4">
         <f>VLOOKUP(A8,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C8" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D8" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E8" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F8" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>38433</v>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>38335</v>
       </c>
       <c r="B9" s="4">
         <f>VLOOKUP(A9,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>2.75E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D9" s="2">
-        <v>2.75E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="E9" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F9" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>38475</v>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>38385</v>
       </c>
       <c r="B10" s="4">
         <f>VLOOKUP(A10,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C10" s="2">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E10" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F10" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>38533</v>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>38433</v>
       </c>
       <c r="B11" s="4">
         <f>VLOOKUP(A11,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>3.2500000000000001E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="D11" s="2">
-        <v>3.2500000000000001E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="E11" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F11" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>38573</v>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>38475</v>
       </c>
       <c r="B12" s="4">
         <f>VLOOKUP(A12,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C12" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D12" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E12" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F12" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>38615</v>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>38533</v>
       </c>
       <c r="B13" s="4">
         <f>VLOOKUP(A13,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C13" s="2">
-        <v>3.7499999999999999E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="D13" s="2">
-        <v>3.7499999999999999E-2</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="E13" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F13" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>38657</v>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>38573</v>
       </c>
       <c r="B14" s="4">
         <f>VLOOKUP(A14,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C14" s="2">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D14" s="2">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E14" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F14" s="2">
-        <f>25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>38699</v>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>38615</v>
       </c>
       <c r="B15" s="4">
         <f>VLOOKUP(A15,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>4.2500000000000003E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="D15" s="2">
-        <v>4.2500000000000003E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:F19" si="0">25/10000</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>38748</v>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>38657</v>
       </c>
       <c r="B16" s="4">
         <f>VLOOKUP(A16,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C16" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D16" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
@@ -5187,200 +5210,213 @@
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>38804</v>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>38699</v>
       </c>
       <c r="B17" s="4">
         <f>VLOOKUP(A17,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C17" s="2">
-        <v>4.7500000000000001E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="D17" s="2">
-        <v>4.7500000000000001E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E17:F21" si="1">25/10000</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>38847</v>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>38748</v>
       </c>
       <c r="B18" s="4">
         <f>VLOOKUP(A18,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D18" s="2">
-        <v>0.05</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>38897</v>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>38804</v>
       </c>
       <c r="B19" s="4">
         <f>VLOOKUP(A19,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C19" s="2">
-        <v>5.2499999999999998E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="D19" s="2">
-        <v>5.2499999999999998E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>39343</v>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>38847</v>
       </c>
       <c r="B20" s="4">
         <f>VLOOKUP(A20,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C20" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>38897</v>
+      </c>
+      <c r="B21" s="4">
+        <f>VLOOKUP(A21,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>39343</v>
+      </c>
+      <c r="B22" s="4">
+        <f>VLOOKUP(A22,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D22" s="2">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E22" s="2">
         <f>-50/10000</f>
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F22" s="2">
         <f>-50/10000</f>
         <v>-5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>39386</v>
       </c>
-      <c r="B21" s="4">
-        <f>VLOOKUP(A21,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B23" s="4">
+        <f>VLOOKUP(A23,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D23" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E23" s="2">
         <f>-25/10000</f>
         <v>-2.5000000000000001E-3</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F23" s="2">
         <f>-25/10000</f>
         <v>-2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>39427</v>
       </c>
-      <c r="B22" s="4">
-        <f>VLOOKUP(A22,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B24" s="4">
+        <f>VLOOKUP(A24,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D24" s="2">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E24" s="2">
         <f>-25/10000</f>
         <v>-2.5000000000000001E-3</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F24" s="2">
         <f>-25/10000</f>
         <v>-2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>39469</v>
-      </c>
-      <c r="B23" s="4">
-        <f>VLOOKUP(A23,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D23" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>-7.4999999999999997E-3</v>
-      </c>
-      <c r="F23" s="2">
-        <v>-7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>39477</v>
-      </c>
-      <c r="B24" s="4">
-        <f>VLOOKUP(A24,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="E24" s="2">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="F24" s="2">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>39525</v>
       </c>
       <c r="B25" s="4">
         <f>VLOOKUP(A25,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>2.2499999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D25" s="2">
-        <v>2.2499999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E25" s="2">
         <v>-7.4999999999999997E-3</v>
@@ -5388,146 +5424,153 @@
       <c r="F25" s="2">
         <v>-7.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>39568</v>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>39477</v>
       </c>
       <c r="B26" s="4">
         <f>VLOOKUP(A26,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C26" s="2">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="D26" s="2">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="E26" s="2">
-        <v>-2.5000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F26" s="2">
-        <v>-2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>39729</v>
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>39525</v>
       </c>
       <c r="B27" s="4">
         <f>VLOOKUP(A27,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D27" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="E27" s="2">
-        <v>-5.0000000000000001E-3</v>
+        <v>-7.4999999999999997E-3</v>
       </c>
       <c r="F27" s="2">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>39750</v>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>39568</v>
       </c>
       <c r="B28" s="4">
         <f>VLOOKUP(A28,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C28" s="2">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D28" s="2">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E28" s="2">
-        <v>-5.0000000000000001E-3</v>
+        <v>-2.5000000000000001E-3</v>
       </c>
       <c r="F28" s="2">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>39798</v>
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>39729</v>
       </c>
       <c r="B29" s="4">
         <f>VLOOKUP(A29,FOMC_Meetings!$A$1:$F$934,4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D29" s="2">
-        <v>2.5000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E29" s="2">
-        <v>-0.01</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F29" s="2">
-        <v>-7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>42355</v>
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>39750</v>
       </c>
       <c r="B30" s="4">
         <f>VLOOKUP(A30,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C30" s="2">
-        <v>2.5000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D30" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E30" s="2">
-        <v>2.5000000000000001E-3</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="F30" s="2">
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>42719</v>
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>39798</v>
       </c>
       <c r="B31" s="4">
         <f>VLOOKUP(A31,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C31" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2">
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E31" s="2">
-        <v>2.5000000000000001E-3</v>
+        <v>-0.01</v>
       </c>
       <c r="F31" s="2">
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>42810</v>
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>42355</v>
       </c>
       <c r="B32" s="4">
         <f>VLOOKUP(A32,FOMC_Meetings!$A$1:$F$934,4)</f>
         <v>1</v>
       </c>
       <c r="C32" s="2">
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D32" s="2">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E32" s="2">
         <v>2.5000000000000001E-3</v>
@@ -5535,6 +5578,51 @@
       <c r="F32" s="2">
         <v>2.5000000000000001E-3</v>
       </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>42719</v>
+      </c>
+      <c r="B33" s="4">
+        <f>VLOOKUP(A33,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D33" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>42810</v>
+      </c>
+      <c r="B34" s="4">
+        <f>VLOOKUP(A34,FOMC_Meetings!$A$1:$F$934,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5547,8 +5635,8 @@
   <dimension ref="A1:F934"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A900" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="1" topLeftCell="A902" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A934" sqref="A934"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24246,7 +24334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Implement Naive Bayes and SVM
</commit_message>
<xml_diff>
--- a/data/FED_OpenMarket_Operations.xlsx
+++ b/data/FED_OpenMarket_Operations.xlsx
@@ -4789,7 +4789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5626,7 +5628,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>42901</v>
+        <v>42900</v>
       </c>
       <c r="B35">
         <v>1</v>

</xml_diff>